<commit_message>
Actualización de datos obtenidos el 6 de abril de 2016
</commit_message>
<xml_diff>
--- a/data/metadata/Informe-01-010042-TC-TM.xlsx
+++ b/data/metadata/Informe-01-010042-TC-TM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
   <si>
     <t>Tipo de presupuesto</t>
   </si>
@@ -115,7 +115,7 @@
     <t>ano</t>
   </si>
   <si>
-    <t>iaest-measure:tipo-de-presupuesto</t>
+    <t>iaest-dimension:tipo-de-presupuesto</t>
   </si>
   <si>
     <t>null</t>
@@ -133,7 +133,7 @@
     <t>iaest-measure:pasivos-financieros</t>
   </si>
   <si>
-    <t>iaest-measure:estado-de-la-informacion</t>
+    <t>iaest-dimension:estado-de-la-informacion</t>
   </si>
   <si>
     <t>iaest-measure:ingresos-patrimoniales</t>
@@ -160,13 +160,13 @@
     <t>sdmx-dimension:refPeriod</t>
   </si>
   <si>
+    <t>dim</t>
+  </si>
+  <si>
     <t>medida</t>
   </si>
   <si>
-    <t>dim</t>
-  </si>
-  <si>
-    <t>xsd:string</t>
+    <t>skos:Concept</t>
   </si>
   <si>
     <t>xsd:double</t>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>xsd:date</t>
+  </si>
+  <si>
+    <t>mapping-tipo-de-presupuesto.xlsx</t>
+  </si>
+  <si>
+    <t>mapping-estado-de-la-informacion.xlsx</t>
   </si>
 </sst>
 </file>
@@ -405,49 +411,49 @@
         <v>35</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>49</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>35</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5">
@@ -501,6 +507,14 @@
       </c>
       <c r="Q5" s="1" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>